<commit_message>
change to use rmtr account number for validation
</commit_message>
<xml_diff>
--- a/docs/EMAMIP_STD_API_SRS_Template_V_1 1.xlsx
+++ b/docs/EMAMIP_STD_API_SRS_Template_V_1 1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\emami-paper-bank-api\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3A2A0B-71AB-41D2-85AA-FD7CAC08FBEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Changes" sheetId="1" r:id="rId1"/>
@@ -36,7 +42,6 @@
     <definedName name="Yes_No">Data_Validation!$B$13:$B$14</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -46,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="141">
   <si>
     <t>Sr no</t>
   </si>
@@ -469,32 +474,17 @@
     <t>NEFT</t>
   </si>
   <si>
-    <t>N01234567890</t>
-  </si>
-  <si>
-    <t>N01234567891</t>
-  </si>
-  <si>
-    <t>N01234567892</t>
-  </si>
-  <si>
-    <t>N01234567893</t>
-  </si>
-  <si>
-    <t>N01234567894</t>
-  </si>
-  <si>
-    <t>N01234567895</t>
+    <t>System Generated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1082,12 +1072,12 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="5"/>
-    <cellStyle name="Hyperlink 3" xfId="10"/>
+    <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Hyperlink 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="6"/>
-    <cellStyle name="Normal 4" xfId="11"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 4" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1171,7 +1161,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Data_Validation"/>
@@ -1184,7 +1174,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Data_Validation"/>
@@ -1197,7 +1187,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="STD_API_SRS_Template_V_1.1"/>
@@ -2290,14 +2280,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.625" style="16" customWidth="1"/>
     <col min="2" max="2" width="5.375" style="16" bestFit="1" customWidth="1"/>
@@ -2314,7 +2304,7 @@
     <col min="257" max="16384" width="10.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="19" t="s">
         <v>71</v>
@@ -2347,7 +2337,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2356,7 +2346,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="29.1" customHeight="1">
+    <row r="4" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="17" t="s">
         <v>0</v>
@@ -2377,7 +2367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="25">
         <v>1</v>
@@ -2396,7 +2386,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="15.75">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
@@ -2405,7 +2395,7 @@
       <c r="F6" s="28"/>
       <c r="G6" s="33"/>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="18"/>
       <c r="C7" s="15"/>
@@ -2414,7 +2404,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="28"/>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2423,7 +2413,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2434,16 +2424,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" location="Flow!A1" display="Flow"/>
-    <hyperlink ref="C2" location="'Ecol Apps'!A1" display="E-Col_Apps"/>
-    <hyperlink ref="D2" location="WebServices!A1" display="WebServices"/>
-    <hyperlink ref="E2" location="'Customer_Setup (RIL)'!A1" display="Customer_Setup"/>
-    <hyperlink ref="H2" location="'Notification Req-Res Format'!A1" display="Notification Req-Res Format"/>
-    <hyperlink ref="I2" location="'Notification Req-Res XML_JSON'!A1" display="Notification Req-Res XML_JSON"/>
-    <hyperlink ref="J2" location="'Service Test Cases'!A1" display="Service Test Cases"/>
-    <hyperlink ref="K2" location="'SC Test Cases'!A1" display="SC Test Cases"/>
-    <hyperlink ref="F2" location="'Notification Req-Res Format'!A1" display="Validation Req-Res Format"/>
-    <hyperlink ref="G2" location="'Notification Req-Res XML_JSON'!A1" display="Notification Req-Res XML_JSON"/>
+    <hyperlink ref="B2" location="Flow!A1" display="Flow" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" location="'Ecol Apps'!A1" display="E-Col_Apps" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" location="WebServices!A1" display="WebServices" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" location="'Customer_Setup (RIL)'!A1" display="Customer_Setup" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H2" location="'Notification Req-Res Format'!A1" display="Notification Req-Res Format" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I2" location="'Notification Req-Res XML_JSON'!A1" display="Notification Req-Res XML_JSON" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J2" location="'Service Test Cases'!A1" display="Service Test Cases" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="K2" location="'SC Test Cases'!A1" display="SC Test Cases" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F2" location="'Notification Req-Res Format'!A1" display="Validation Req-Res Format" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G2" location="'Notification Req-Res XML_JSON'!A1" display="Notification Req-Res XML_JSON" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -2454,14 +2444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E41"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.5" style="38" customWidth="1"/>
     <col min="2" max="2" width="35" style="38" bestFit="1" customWidth="1"/>
@@ -2471,24 +2461,24 @@
     <col min="6" max="16384" width="10.875" style="38"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
     </row>
-    <row r="6" spans="1:5" ht="16.5">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B6" s="41" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="40"/>
       <c r="D6" s="39"/>
     </row>
-    <row r="7" spans="1:5" ht="16.5">
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
         <v>10</v>
       </c>
@@ -2502,7 +2492,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="31.5">
+    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
         <v>10</v>
       </c>
@@ -2516,7 +2506,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5">
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="39"/>
       <c r="B9" s="79" t="s">
         <v>29</v>
@@ -2529,7 +2519,7 @@
       </c>
       <c r="E9" s="42"/>
     </row>
-    <row r="10" spans="1:5" ht="16.5">
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
         <v>10</v>
       </c>
@@ -2544,7 +2534,7 @@
       </c>
       <c r="E10" s="42"/>
     </row>
-    <row r="11" spans="1:5" ht="16.5">
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="38" t="s">
         <v>27</v>
@@ -2557,13 +2547,13 @@
       </c>
       <c r="E11" s="42"/>
     </row>
-    <row r="12" spans="1:5" ht="16.5">
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
       <c r="B12" s="40"/>
       <c r="D12" s="39"/>
       <c r="E12" s="42"/>
     </row>
-    <row r="13" spans="1:5" ht="16.5">
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="41" t="s">
         <v>103</v>
@@ -2572,7 +2562,7 @@
       <c r="D13" s="39"/>
       <c r="E13" s="42"/>
     </row>
-    <row r="14" spans="1:5" ht="16.5">
+    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="42" t="s">
         <v>12</v>
@@ -2583,7 +2573,7 @@
       <c r="D14" s="39"/>
       <c r="E14" s="42"/>
     </row>
-    <row r="15" spans="1:5" ht="16.5">
+    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="42" t="s">
         <v>14</v>
@@ -2596,7 +2586,7 @@
       </c>
       <c r="E15" s="42"/>
     </row>
-    <row r="16" spans="1:5" ht="16.5">
+    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="42" t="s">
         <v>16</v>
@@ -2607,7 +2597,7 @@
       <c r="D16" s="76"/>
       <c r="E16" s="42"/>
     </row>
-    <row r="17" spans="1:5" ht="16.5">
+    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="42" t="s">
         <v>19</v>
@@ -2618,7 +2608,7 @@
       <c r="D17" s="76"/>
       <c r="E17" s="42"/>
     </row>
-    <row r="18" spans="1:5" ht="16.5">
+    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="42" t="s">
         <v>22</v>
@@ -2629,7 +2619,7 @@
       <c r="D18" s="76"/>
       <c r="E18" s="42"/>
     </row>
-    <row r="19" spans="1:5" ht="16.5">
+    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="42" t="s">
         <v>23</v>
@@ -2640,7 +2630,7 @@
       <c r="D19" s="76"/>
       <c r="E19" s="42"/>
     </row>
-    <row r="20" spans="1:5" ht="16.5">
+    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="42" t="s">
         <v>20</v>
@@ -2651,7 +2641,7 @@
       <c r="D20" s="39"/>
       <c r="E20" s="42"/>
     </row>
-    <row r="21" spans="1:5" ht="16.5">
+    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B21" s="72" t="s">
         <v>28</v>
       </c>
@@ -2661,7 +2651,7 @@
       <c r="D21" s="77"/>
       <c r="E21" s="42"/>
     </row>
-    <row r="22" spans="1:5" ht="16.5">
+    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B22" s="72" t="s">
         <v>24</v>
       </c>
@@ -2671,7 +2661,7 @@
       <c r="D22" s="77"/>
       <c r="E22" s="42"/>
     </row>
-    <row r="23" spans="1:5" ht="16.5">
+    <row r="23" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
       <c r="B23" s="72" t="s">
         <v>32</v>
@@ -2682,7 +2672,7 @@
       <c r="D23" s="77"/>
       <c r="E23" s="42"/>
     </row>
-    <row r="24" spans="1:5" ht="16.5">
+    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
       <c r="B24" s="72" t="s">
         <v>33</v>
@@ -2693,7 +2683,7 @@
       <c r="D24" s="77"/>
       <c r="E24" s="42"/>
     </row>
-    <row r="25" spans="1:5" ht="16.5">
+    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="72" t="s">
         <v>36</v>
@@ -2704,7 +2694,7 @@
       <c r="D25" s="77"/>
       <c r="E25" s="42"/>
     </row>
-    <row r="26" spans="1:5" ht="16.5">
+    <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="47"/>
       <c r="B26" s="72" t="s">
         <v>38</v>
@@ -2715,7 +2705,7 @@
       <c r="D26" s="77"/>
       <c r="E26" s="42"/>
     </row>
-    <row r="27" spans="1:5" ht="16.5">
+    <row r="27" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
       <c r="B27" s="72" t="s">
         <v>39</v>
@@ -2726,7 +2716,7 @@
       <c r="D27" s="77"/>
       <c r="E27" s="42"/>
     </row>
-    <row r="28" spans="1:5" ht="16.5">
+    <row r="28" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
         <v>10</v>
       </c>
@@ -2739,14 +2729,14 @@
       <c r="D28" s="77"/>
       <c r="E28" s="42"/>
     </row>
-    <row r="29" spans="1:5" ht="16.5">
+    <row r="29" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="41"/>
       <c r="C29" s="40"/>
       <c r="D29" s="39"/>
       <c r="E29" s="42"/>
     </row>
-    <row r="30" spans="1:5" ht="16.5">
+    <row r="30" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
       <c r="B30" s="41" t="s">
         <v>104</v>
@@ -2755,7 +2745,7 @@
       <c r="D30" s="39"/>
       <c r="E30" s="42"/>
     </row>
-    <row r="31" spans="1:5" ht="16.5">
+    <row r="31" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="47"/>
       <c r="B31" s="72" t="s">
         <v>35</v>
@@ -2766,7 +2756,7 @@
       <c r="D31" s="39"/>
       <c r="E31" s="42"/>
     </row>
-    <row r="32" spans="1:5" ht="16.5">
+    <row r="32" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="47"/>
       <c r="B32" s="72" t="s">
         <v>37</v>
@@ -2777,7 +2767,7 @@
       <c r="D32" s="39"/>
       <c r="E32" s="42"/>
     </row>
-    <row r="33" spans="1:5" ht="16.5">
+    <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="47"/>
       <c r="B33" s="73" t="s">
         <v>26</v>
@@ -2786,56 +2776,56 @@
       <c r="D33" s="39"/>
       <c r="E33" s="42"/>
     </row>
-    <row r="34" spans="1:5" ht="16.5">
+    <row r="34" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
       <c r="B34" s="41"/>
       <c r="C34" s="40"/>
       <c r="D34" s="39"/>
       <c r="E34" s="42"/>
     </row>
-    <row r="35" spans="1:5" ht="16.5">
+    <row r="35" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="47"/>
       <c r="B35" s="41"/>
       <c r="C35" s="40"/>
       <c r="D35" s="39"/>
       <c r="E35" s="42"/>
     </row>
-    <row r="36" spans="1:5" ht="16.5">
+    <row r="36" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="47"/>
       <c r="B36" s="41"/>
       <c r="C36" s="40"/>
       <c r="D36" s="39"/>
       <c r="E36" s="42"/>
     </row>
-    <row r="37" spans="1:5" ht="16.5">
+    <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
       <c r="B37" s="41"/>
       <c r="C37" s="40"/>
       <c r="D37" s="39"/>
       <c r="E37" s="42"/>
     </row>
-    <row r="38" spans="1:5" ht="16.5">
+    <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="47"/>
       <c r="B38" s="41"/>
       <c r="C38" s="40"/>
       <c r="D38" s="39"/>
       <c r="E38" s="42"/>
     </row>
-    <row r="39" spans="1:5" ht="16.5">
+    <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="47"/>
       <c r="B39" s="41"/>
       <c r="C39" s="40"/>
       <c r="D39" s="39"/>
       <c r="E39" s="42"/>
     </row>
-    <row r="40" spans="1:5" ht="16.5">
+    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="47"/>
       <c r="B40" s="41"/>
       <c r="C40" s="40"/>
       <c r="D40" s="39"/>
       <c r="E40" s="42"/>
     </row>
-    <row r="41" spans="1:5" ht="16.5">
+    <row r="41" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
       <c r="B41" s="41"/>
       <c r="C41" s="40"/>
@@ -2844,37 +2834,37 @@
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21">
-      <formula1>[3]!Lookup_File_Upload_Treatment</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>STD_API_SRS_Template_V_1.1.xlsx!Lookup_File_Upload_Treatment</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14">
-      <formula1>[3]!Validate_Txn_Dt</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{00000000-0002-0000-0100-000001000000}">
+      <formula1>STD_API_SRS_Template_V_1.1.xlsx!Validate_Txn_Dt</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C19 C31:C32 C23 C25 C27">
-      <formula1>[3]!Yes_No</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C19 C31:C32 C23 C25 C27" xr:uid="{00000000-0002-0000-0100-000002000000}">
+      <formula1>STD_API_SRS_Template_V_1.1.xlsx!Yes_No</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22 C24 C26">
-      <formula1>[3]!Account_Token</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22 C24 C26" xr:uid="{00000000-0002-0000-0100-000003000000}">
+      <formula1>STD_API_SRS_Template_V_1.1.xlsx!Account_Token</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15">
-      <formula1>[3]!Validate_Txn_Amt</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{00000000-0002-0000-0100-000004000000}">
+      <formula1>STD_API_SRS_Template_V_1.1.xlsx!Validate_Txn_Amt</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>"On Credit, On Return, None, Always"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>"ECSTDX01, ECSTDJ01"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A2" location="Changes!A1" display="Back to route"/>
+    <hyperlink ref="A2" location="Changes!A1" display="Back to route" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>Data_Validation!$B$2:$B$5</xm:f>
           </x14:formula1>
@@ -2887,14 +2877,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.625" style="65" customWidth="1"/>
     <col min="2" max="2" width="26" style="65" customWidth="1"/>
@@ -2907,7 +2897,7 @@
     <col min="257" max="16384" width="10.625" style="52"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>70</v>
       </c>
@@ -2918,7 +2908,7 @@
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
     </row>
-    <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
@@ -2927,7 +2917,7 @@
       <c r="F3" s="52"/>
       <c r="G3" s="52"/>
     </row>
-    <row r="4" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="53"/>
       <c r="B4" s="54" t="s">
         <v>101</v>
@@ -2944,7 +2934,7 @@
       <c r="F4" s="52"/>
       <c r="G4" s="52"/>
     </row>
-    <row r="5" spans="1:7" ht="31.5">
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="55"/>
       <c r="B5" s="56" t="s">
         <v>92</v>
@@ -2961,7 +2951,7 @@
       <c r="F5" s="52"/>
       <c r="G5" s="52"/>
     </row>
-    <row r="6" spans="1:7" ht="18" customHeight="1">
+    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="55"/>
       <c r="B6" s="74" t="s">
         <v>91</v>
@@ -2978,7 +2968,7 @@
       <c r="F6" s="52"/>
       <c r="G6" s="52"/>
     </row>
-    <row r="7" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="55"/>
       <c r="B7" s="61" t="s">
         <v>78</v>
@@ -2993,7 +2983,7 @@
       <c r="F7" s="52"/>
       <c r="G7" s="52"/>
     </row>
-    <row r="8" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="55"/>
       <c r="B8" s="61" t="s">
         <v>7</v>
@@ -3008,7 +2998,7 @@
       <c r="F8" s="52"/>
       <c r="G8" s="52"/>
     </row>
-    <row r="9" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="55"/>
       <c r="B9" s="61" t="s">
         <v>97</v>
@@ -3021,7 +3011,7 @@
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75">
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="55"/>
       <c r="B10" s="56" t="s">
         <v>98</v>
@@ -3034,7 +3024,7 @@
       <c r="F10" s="52"/>
       <c r="G10" s="52"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="52"/>
       <c r="B11" s="62"/>
       <c r="C11" s="52"/>
@@ -3043,7 +3033,7 @@
       <c r="F11" s="52"/>
       <c r="G11" s="52"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="52"/>
       <c r="B12" s="62"/>
       <c r="C12" s="52"/>
@@ -3052,7 +3042,7 @@
       <c r="F12" s="52"/>
       <c r="G12" s="52"/>
     </row>
-    <row r="13" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52"/>
       <c r="B13" s="52"/>
       <c r="C13" s="52"/>
@@ -3063,14 +3053,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:D5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:D5" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"ECSTDX01, ECSTDJ01"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A2" location="Changes!A1" display="Back to route"/>
-    <hyperlink ref="C7" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="A2" location="Changes!A1" display="Back to route" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3081,14 +3071,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.875" style="49"/>
     <col min="2" max="2" width="24.625" style="49" customWidth="1"/>
@@ -3096,7 +3086,7 @@
     <col min="4" max="4" width="23.375" style="49" customWidth="1"/>
     <col min="5" max="5" width="20.375" style="49" customWidth="1"/>
     <col min="6" max="6" width="19.5" style="49" customWidth="1"/>
-    <col min="7" max="7" width="18.125" style="49" customWidth="1"/>
+    <col min="7" max="7" width="21.75" style="49" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.375" style="49" customWidth="1"/>
     <col min="9" max="9" width="23" style="49" customWidth="1"/>
     <col min="10" max="10" width="18.625" style="49" bestFit="1" customWidth="1"/>
@@ -3108,32 +3098,32 @@
     <col min="16" max="16384" width="10.875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C1" s="49" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C2" s="49" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C3" s="49" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C4" s="49" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C5" s="49" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="2:14" s="48" customFormat="1">
+    <row r="7" spans="2:14" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="50" t="s">
         <v>112</v>
       </c>
@@ -3166,7 +3156,7 @@
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="75" t="s">
         <v>109</v>
       </c>
@@ -3192,10 +3182,10 @@
         <v>100</v>
       </c>
       <c r="J8" s="49">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14">
+        <v>123456780</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="75" t="s">
         <v>110</v>
       </c>
@@ -3212,7 +3202,7 @@
         <v>139</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H9" s="87">
         <v>43784.728668981479</v>
@@ -3221,10 +3211,10 @@
         <v>100</v>
       </c>
       <c r="J9" s="49">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14">
+        <v>123456781</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="75" t="s">
         <v>111</v>
       </c>
@@ -3241,7 +3231,7 @@
         <v>139</v>
       </c>
       <c r="G10" s="49" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H10" s="87">
         <v>43784.728668981479</v>
@@ -3250,10 +3240,10 @@
         <v>100</v>
       </c>
       <c r="J10" s="49">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14">
+        <v>123456782</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="49" t="s">
         <v>88</v>
       </c>
@@ -3270,7 +3260,7 @@
         <v>139</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H11" s="87">
         <v>43784.728668981479</v>
@@ -3279,10 +3269,10 @@
         <v>100</v>
       </c>
       <c r="J11" s="49">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
+        <v>123456783</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="49" t="s">
         <v>69</v>
       </c>
@@ -3299,7 +3289,7 @@
         <v>139</v>
       </c>
       <c r="G12" s="49" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H12" s="87">
         <v>43784.728668981479</v>
@@ -3308,10 +3298,10 @@
         <v>100</v>
       </c>
       <c r="J12" s="49">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14">
+        <v>123456784</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="49" t="s">
         <v>87</v>
       </c>
@@ -3328,7 +3318,7 @@
         <v>139</v>
       </c>
       <c r="G13" s="49" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H13" s="87">
         <v>43784.728668981479</v>
@@ -3337,10 +3327,10 @@
         <v>100</v>
       </c>
       <c r="J13" s="49">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
+        <v>123456785</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="71" t="s">
         <v>128</v>
       </c>
@@ -3369,14 +3359,14 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="84" t="s">
         <v>135</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F35" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"NEFT, RTGS, IMPS, UPI"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3386,14 +3376,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.875" style="49"/>
     <col min="2" max="2" width="24.625" style="49" customWidth="1"/>
@@ -3413,22 +3403,22 @@
     <col min="16" max="16384" width="10.875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C1" s="49" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C2" s="49" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C3" s="49" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:14" s="48" customFormat="1">
+    <row r="5" spans="2:14" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="50" t="s">
         <v>112</v>
       </c>
@@ -3461,7 +3451,7 @@
       <c r="M5" s="50"/>
       <c r="N5" s="50"/>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="75" t="s">
         <v>109</v>
       </c>
@@ -3469,7 +3459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="75" t="s">
         <v>110</v>
       </c>
@@ -3477,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="75" t="s">
         <v>111</v>
       </c>
@@ -3485,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="49" t="s">
         <v>8</v>
       </c>
@@ -3493,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="49" t="s">
         <v>86</v>
       </c>
@@ -3501,7 +3491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="71" t="s">
         <v>128</v>
       </c>
@@ -3530,17 +3520,17 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D15" s="84" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D16" s="48"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F32" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"NEFT, RTGS, IMPS, UPI"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3550,12 +3540,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.625" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.875" style="23"/>
@@ -3563,7 +3553,7 @@
     <col min="5" max="16384" width="10.875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5">
+    <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>40</v>
       </c>
@@ -3571,7 +3561,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="21" t="s">
         <v>13</v>
       </c>
@@ -3579,7 +3569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
         <v>21</v>
       </c>
@@ -3587,7 +3577,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
         <v>43</v>
       </c>
@@ -3595,7 +3585,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="36" t="s">
         <v>85</v>
       </c>
@@ -3603,7 +3593,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>45</v>
       </c>
@@ -3611,7 +3601,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
         <v>13</v>
       </c>
@@ -3619,7 +3609,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="21" t="s">
         <v>15</v>
       </c>
@@ -3627,7 +3617,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="21" t="s">
         <v>49</v>
       </c>
@@ -3635,7 +3625,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="21" t="s">
         <v>51</v>
       </c>
@@ -3643,12 +3633,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>54</v>
       </c>
@@ -3656,123 +3646,123 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="21"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="21"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B28" s="21"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="21"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" s="21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" s="21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16.5">
+    <row r="39" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B39" s="22" t="s">
         <v>34</v>
       </c>

</xml_diff>